<commit_message>
Update with re-org and RA instructions 2x
</commit_message>
<xml_diff>
--- a/js/earhart-fellows/Miscellaneous/Mont Pelerin Society Directory 2010.xlsx
+++ b/js/earhart-fellows/Miscellaneous/Mont Pelerin Society Directory 2010.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="4824" tabRatio="204" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="4824" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDFTables.com" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -5983,7 +5983,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -6332,7 +6332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2641"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B39" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -17794,6 +17794,474 @@
     <row r="2641" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="480">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A242:B242"/>
+    <mergeCell ref="A243:B243"/>
+    <mergeCell ref="A292:B292"/>
+    <mergeCell ref="A293:B293"/>
+    <mergeCell ref="A342:B342"/>
+    <mergeCell ref="A343:B343"/>
+    <mergeCell ref="A392:B392"/>
+    <mergeCell ref="A393:B393"/>
+    <mergeCell ref="A394:B394"/>
+    <mergeCell ref="A395:B395"/>
+    <mergeCell ref="A396:B396"/>
+    <mergeCell ref="A397:B397"/>
+    <mergeCell ref="A398:B398"/>
+    <mergeCell ref="A399:B399"/>
+    <mergeCell ref="A400:B400"/>
+    <mergeCell ref="A401:B401"/>
+    <mergeCell ref="A402:B402"/>
+    <mergeCell ref="A403:B403"/>
+    <mergeCell ref="A404:B404"/>
+    <mergeCell ref="A405:B405"/>
+    <mergeCell ref="A406:B406"/>
+    <mergeCell ref="A407:B407"/>
+    <mergeCell ref="A408:B408"/>
+    <mergeCell ref="A409:B409"/>
+    <mergeCell ref="A410:B410"/>
+    <mergeCell ref="A411:B411"/>
+    <mergeCell ref="A412:B412"/>
+    <mergeCell ref="A413:B413"/>
+    <mergeCell ref="A414:B414"/>
+    <mergeCell ref="A415:B415"/>
+    <mergeCell ref="A416:B416"/>
+    <mergeCell ref="A417:B417"/>
+    <mergeCell ref="A418:B418"/>
+    <mergeCell ref="A419:B419"/>
+    <mergeCell ref="A420:B420"/>
+    <mergeCell ref="A421:B421"/>
+    <mergeCell ref="A422:B422"/>
+    <mergeCell ref="A423:B423"/>
+    <mergeCell ref="A424:B424"/>
+    <mergeCell ref="A425:B425"/>
+    <mergeCell ref="A426:B426"/>
+    <mergeCell ref="A427:B427"/>
+    <mergeCell ref="A428:B428"/>
+    <mergeCell ref="A429:B429"/>
+    <mergeCell ref="A430:B430"/>
+    <mergeCell ref="A431:B431"/>
+    <mergeCell ref="A442:B442"/>
+    <mergeCell ref="A443:B443"/>
+    <mergeCell ref="A492:B492"/>
+    <mergeCell ref="A493:B493"/>
+    <mergeCell ref="A542:B542"/>
+    <mergeCell ref="A543:B543"/>
+    <mergeCell ref="A592:B592"/>
+    <mergeCell ref="A593:B593"/>
+    <mergeCell ref="A642:B642"/>
+    <mergeCell ref="A643:B643"/>
+    <mergeCell ref="A692:B692"/>
+    <mergeCell ref="A693:B693"/>
+    <mergeCell ref="A742:B742"/>
+    <mergeCell ref="A743:B743"/>
+    <mergeCell ref="A792:B792"/>
+    <mergeCell ref="A793:B793"/>
+    <mergeCell ref="A842:B842"/>
+    <mergeCell ref="A843:B843"/>
+    <mergeCell ref="A844:B844"/>
+    <mergeCell ref="A845:B845"/>
+    <mergeCell ref="A846:B846"/>
+    <mergeCell ref="A847:B847"/>
+    <mergeCell ref="A848:B848"/>
+    <mergeCell ref="A849:B849"/>
+    <mergeCell ref="A850:B850"/>
+    <mergeCell ref="A851:B851"/>
+    <mergeCell ref="A852:B852"/>
+    <mergeCell ref="A853:B853"/>
+    <mergeCell ref="A854:B854"/>
+    <mergeCell ref="A855:B855"/>
+    <mergeCell ref="A856:B856"/>
+    <mergeCell ref="A857:B857"/>
+    <mergeCell ref="A858:B858"/>
+    <mergeCell ref="A859:B859"/>
+    <mergeCell ref="A860:B860"/>
+    <mergeCell ref="A861:B861"/>
+    <mergeCell ref="A862:B862"/>
+    <mergeCell ref="A863:B863"/>
+    <mergeCell ref="A864:B864"/>
+    <mergeCell ref="A865:B865"/>
+    <mergeCell ref="A866:B866"/>
+    <mergeCell ref="A867:B867"/>
+    <mergeCell ref="A868:B868"/>
+    <mergeCell ref="A869:B869"/>
+    <mergeCell ref="A870:B870"/>
+    <mergeCell ref="A871:B871"/>
+    <mergeCell ref="A872:B872"/>
+    <mergeCell ref="A873:B873"/>
+    <mergeCell ref="A892:B892"/>
+    <mergeCell ref="A893:B893"/>
+    <mergeCell ref="A942:B942"/>
+    <mergeCell ref="A943:B943"/>
+    <mergeCell ref="A992:B992"/>
+    <mergeCell ref="A993:B993"/>
+    <mergeCell ref="A1042:B1042"/>
+    <mergeCell ref="A1043:B1043"/>
+    <mergeCell ref="A1092:B1092"/>
+    <mergeCell ref="A1093:B1093"/>
+    <mergeCell ref="A1142:B1142"/>
+    <mergeCell ref="A1143:B1143"/>
+    <mergeCell ref="A1192:B1192"/>
+    <mergeCell ref="A1193:B1193"/>
+    <mergeCell ref="A1242:B1242"/>
+    <mergeCell ref="A1243:B1243"/>
+    <mergeCell ref="A1292:B1292"/>
+    <mergeCell ref="A1293:B1293"/>
+    <mergeCell ref="A1342:B1342"/>
+    <mergeCell ref="A1343:B1343"/>
+    <mergeCell ref="A1392:B1392"/>
+    <mergeCell ref="A1393:B1393"/>
+    <mergeCell ref="A1442:B1442"/>
+    <mergeCell ref="A1443:B1443"/>
+    <mergeCell ref="A1492:B1492"/>
+    <mergeCell ref="A1493:B1493"/>
+    <mergeCell ref="A1542:B1542"/>
+    <mergeCell ref="A1543:B1543"/>
+    <mergeCell ref="A1544:B1544"/>
+    <mergeCell ref="A1545:B1545"/>
+    <mergeCell ref="A1546:B1546"/>
+    <mergeCell ref="A1547:B1547"/>
+    <mergeCell ref="A1548:B1548"/>
+    <mergeCell ref="A1549:B1549"/>
+    <mergeCell ref="A1550:B1550"/>
+    <mergeCell ref="A1551:B1551"/>
+    <mergeCell ref="A1552:B1552"/>
+    <mergeCell ref="A1553:B1553"/>
+    <mergeCell ref="A1554:B1554"/>
+    <mergeCell ref="A1555:B1555"/>
+    <mergeCell ref="A1556:B1556"/>
+    <mergeCell ref="A1557:B1557"/>
+    <mergeCell ref="A1558:B1558"/>
+    <mergeCell ref="A1559:B1559"/>
+    <mergeCell ref="A1560:B1560"/>
+    <mergeCell ref="A1561:B1561"/>
+    <mergeCell ref="A1562:B1562"/>
+    <mergeCell ref="A1563:B1563"/>
+    <mergeCell ref="A1564:B1564"/>
+    <mergeCell ref="A1565:B1565"/>
+    <mergeCell ref="A1566:B1566"/>
+    <mergeCell ref="A1567:B1567"/>
+    <mergeCell ref="A1568:B1568"/>
+    <mergeCell ref="A1569:B1569"/>
+    <mergeCell ref="A1570:B1570"/>
+    <mergeCell ref="A1571:B1571"/>
+    <mergeCell ref="A1572:B1572"/>
+    <mergeCell ref="A1573:B1573"/>
+    <mergeCell ref="A1574:B1574"/>
+    <mergeCell ref="A1575:B1575"/>
+    <mergeCell ref="A1576:B1576"/>
+    <mergeCell ref="A1577:B1577"/>
+    <mergeCell ref="A1578:B1578"/>
+    <mergeCell ref="A1579:B1579"/>
+    <mergeCell ref="A1580:B1580"/>
+    <mergeCell ref="A1581:B1581"/>
+    <mergeCell ref="A1582:B1582"/>
+    <mergeCell ref="A1583:B1583"/>
+    <mergeCell ref="A1584:B1584"/>
+    <mergeCell ref="A1585:B1585"/>
+    <mergeCell ref="A1592:B1592"/>
+    <mergeCell ref="A1593:B1593"/>
+    <mergeCell ref="A1642:B1642"/>
+    <mergeCell ref="A1643:B1643"/>
+    <mergeCell ref="A1644:B1644"/>
+    <mergeCell ref="A1645:B1645"/>
+    <mergeCell ref="A1646:B1646"/>
+    <mergeCell ref="A1647:B1647"/>
+    <mergeCell ref="A1648:B1648"/>
+    <mergeCell ref="A1649:B1649"/>
+    <mergeCell ref="A1650:B1650"/>
+    <mergeCell ref="A1651:B1651"/>
+    <mergeCell ref="A1652:B1652"/>
+    <mergeCell ref="A1653:B1653"/>
+    <mergeCell ref="A1654:B1654"/>
+    <mergeCell ref="A1655:B1655"/>
+    <mergeCell ref="A1656:B1656"/>
+    <mergeCell ref="A1657:B1657"/>
+    <mergeCell ref="A1658:B1658"/>
+    <mergeCell ref="A1659:B1659"/>
+    <mergeCell ref="A1660:B1660"/>
+    <mergeCell ref="A1661:B1661"/>
+    <mergeCell ref="A1662:B1662"/>
+    <mergeCell ref="A1663:B1663"/>
+    <mergeCell ref="A1664:B1664"/>
+    <mergeCell ref="A1665:B1665"/>
+    <mergeCell ref="A1666:B1666"/>
+    <mergeCell ref="A1667:B1667"/>
+    <mergeCell ref="A1668:B1668"/>
+    <mergeCell ref="A1669:B1669"/>
+    <mergeCell ref="A1670:B1670"/>
+    <mergeCell ref="A1671:B1671"/>
+    <mergeCell ref="A1672:B1672"/>
+    <mergeCell ref="A1673:B1673"/>
+    <mergeCell ref="A1674:B1674"/>
+    <mergeCell ref="A1675:B1675"/>
+    <mergeCell ref="A1676:B1676"/>
+    <mergeCell ref="A1677:B1677"/>
+    <mergeCell ref="A1678:B1678"/>
+    <mergeCell ref="A1679:B1679"/>
+    <mergeCell ref="A1680:B1680"/>
+    <mergeCell ref="A1681:B1681"/>
+    <mergeCell ref="A1682:B1682"/>
+    <mergeCell ref="A1683:B1683"/>
+    <mergeCell ref="A1684:B1684"/>
+    <mergeCell ref="A1692:B1692"/>
+    <mergeCell ref="A1693:B1693"/>
+    <mergeCell ref="A1742:B1742"/>
+    <mergeCell ref="A1743:B1743"/>
+    <mergeCell ref="A1744:B1744"/>
+    <mergeCell ref="A1745:B1745"/>
+    <mergeCell ref="A1746:B1746"/>
+    <mergeCell ref="A1747:B1747"/>
+    <mergeCell ref="A1748:B1748"/>
+    <mergeCell ref="A1749:B1749"/>
+    <mergeCell ref="A1750:B1750"/>
+    <mergeCell ref="A1751:B1751"/>
+    <mergeCell ref="A1752:B1752"/>
+    <mergeCell ref="A1753:B1753"/>
+    <mergeCell ref="A1754:B1754"/>
+    <mergeCell ref="A1755:B1755"/>
+    <mergeCell ref="A1756:B1756"/>
+    <mergeCell ref="A1757:B1757"/>
+    <mergeCell ref="A1758:B1758"/>
+    <mergeCell ref="A1759:B1759"/>
+    <mergeCell ref="A1760:B1760"/>
+    <mergeCell ref="A1761:B1761"/>
+    <mergeCell ref="A1762:B1762"/>
+    <mergeCell ref="A1763:B1763"/>
+    <mergeCell ref="A1764:B1764"/>
+    <mergeCell ref="A1765:B1765"/>
+    <mergeCell ref="A1766:B1766"/>
+    <mergeCell ref="A1767:B1767"/>
+    <mergeCell ref="A1792:B1792"/>
+    <mergeCell ref="A1793:B1793"/>
+    <mergeCell ref="A1794:B1794"/>
+    <mergeCell ref="A1795:B1795"/>
+    <mergeCell ref="A1796:B1796"/>
+    <mergeCell ref="A1797:B1797"/>
+    <mergeCell ref="A1798:B1798"/>
+    <mergeCell ref="A1799:B1799"/>
+    <mergeCell ref="A1800:B1800"/>
+    <mergeCell ref="A1801:B1801"/>
+    <mergeCell ref="A1802:B1802"/>
+    <mergeCell ref="A1803:B1803"/>
+    <mergeCell ref="A1804:B1804"/>
+    <mergeCell ref="A1805:B1805"/>
+    <mergeCell ref="A1806:B1806"/>
+    <mergeCell ref="A1807:B1807"/>
+    <mergeCell ref="A1808:B1808"/>
+    <mergeCell ref="A1809:B1809"/>
+    <mergeCell ref="A1810:B1810"/>
+    <mergeCell ref="A1811:B1811"/>
+    <mergeCell ref="A1812:B1812"/>
+    <mergeCell ref="A1813:B1813"/>
+    <mergeCell ref="A1814:B1814"/>
+    <mergeCell ref="A1815:B1815"/>
+    <mergeCell ref="A1816:B1816"/>
+    <mergeCell ref="A1817:B1817"/>
+    <mergeCell ref="A1818:B1818"/>
+    <mergeCell ref="A1819:B1819"/>
+    <mergeCell ref="A1820:B1820"/>
+    <mergeCell ref="A1821:B1821"/>
+    <mergeCell ref="A1822:B1822"/>
+    <mergeCell ref="A1842:B1842"/>
+    <mergeCell ref="A1843:B1843"/>
+    <mergeCell ref="A1892:B1892"/>
+    <mergeCell ref="A1893:B1893"/>
+    <mergeCell ref="A1942:B1942"/>
+    <mergeCell ref="A1943:B1943"/>
+    <mergeCell ref="A1944:B1944"/>
+    <mergeCell ref="A1945:B1945"/>
+    <mergeCell ref="A1946:B1946"/>
+    <mergeCell ref="A1947:B1947"/>
+    <mergeCell ref="A1948:B1948"/>
+    <mergeCell ref="A1949:B1949"/>
+    <mergeCell ref="A1950:B1950"/>
+    <mergeCell ref="A1951:B1951"/>
+    <mergeCell ref="A1952:B1952"/>
+    <mergeCell ref="A1953:B1953"/>
+    <mergeCell ref="A1954:B1954"/>
+    <mergeCell ref="A1955:B1955"/>
+    <mergeCell ref="A1956:B1956"/>
+    <mergeCell ref="A1957:B1957"/>
+    <mergeCell ref="A1958:B1958"/>
+    <mergeCell ref="A1959:B1959"/>
+    <mergeCell ref="A1960:B1960"/>
+    <mergeCell ref="A1961:B1961"/>
+    <mergeCell ref="A1962:B1962"/>
+    <mergeCell ref="A1963:B1963"/>
+    <mergeCell ref="A1964:B1964"/>
+    <mergeCell ref="A1965:B1965"/>
+    <mergeCell ref="A1966:B1966"/>
+    <mergeCell ref="A1967:B1967"/>
+    <mergeCell ref="A1968:B1968"/>
+    <mergeCell ref="A1969:B1969"/>
+    <mergeCell ref="A1970:B1970"/>
+    <mergeCell ref="A1971:B1971"/>
+    <mergeCell ref="A1972:B1972"/>
+    <mergeCell ref="A1973:B1973"/>
+    <mergeCell ref="A1992:B1992"/>
+    <mergeCell ref="A1993:B1993"/>
+    <mergeCell ref="A1994:B1994"/>
+    <mergeCell ref="A1995:B1995"/>
+    <mergeCell ref="A2042:B2042"/>
+    <mergeCell ref="A2043:B2043"/>
+    <mergeCell ref="A2092:B2092"/>
+    <mergeCell ref="A2093:B2093"/>
+    <mergeCell ref="A2094:B2094"/>
+    <mergeCell ref="A2095:B2095"/>
+    <mergeCell ref="A2096:B2096"/>
+    <mergeCell ref="A2097:B2097"/>
+    <mergeCell ref="A2098:B2098"/>
+    <mergeCell ref="A2099:B2099"/>
+    <mergeCell ref="A2100:B2100"/>
+    <mergeCell ref="A2101:B2101"/>
+    <mergeCell ref="A2102:B2102"/>
+    <mergeCell ref="A2103:B2103"/>
+    <mergeCell ref="A2104:B2104"/>
+    <mergeCell ref="A2105:B2105"/>
+    <mergeCell ref="A2142:B2142"/>
+    <mergeCell ref="A2143:B2143"/>
+    <mergeCell ref="A2192:B2192"/>
+    <mergeCell ref="A2193:B2193"/>
+    <mergeCell ref="A2242:B2242"/>
+    <mergeCell ref="A2243:B2243"/>
+    <mergeCell ref="A2244:B2244"/>
+    <mergeCell ref="A2245:B2245"/>
+    <mergeCell ref="A2246:B2246"/>
+    <mergeCell ref="A2247:B2247"/>
+    <mergeCell ref="A2248:B2248"/>
+    <mergeCell ref="A2292:B2292"/>
+    <mergeCell ref="A2293:B2293"/>
+    <mergeCell ref="A2342:B2342"/>
+    <mergeCell ref="A2343:B2343"/>
+    <mergeCell ref="A2392:B2392"/>
+    <mergeCell ref="A2393:B2393"/>
+    <mergeCell ref="A2442:B2442"/>
+    <mergeCell ref="A2443:B2443"/>
+    <mergeCell ref="A2444:B2444"/>
+    <mergeCell ref="A2445:B2445"/>
+    <mergeCell ref="A2446:B2446"/>
+    <mergeCell ref="A2447:B2447"/>
+    <mergeCell ref="A2448:B2448"/>
+    <mergeCell ref="A2449:B2449"/>
+    <mergeCell ref="A2450:B2450"/>
+    <mergeCell ref="A2451:B2451"/>
+    <mergeCell ref="A2452:B2452"/>
+    <mergeCell ref="A2453:B2453"/>
+    <mergeCell ref="A2454:B2454"/>
+    <mergeCell ref="A2455:B2455"/>
+    <mergeCell ref="A2456:B2456"/>
+    <mergeCell ref="A2457:B2457"/>
+    <mergeCell ref="A2458:B2458"/>
+    <mergeCell ref="A2459:B2459"/>
+    <mergeCell ref="A2460:B2460"/>
+    <mergeCell ref="A2461:B2461"/>
+    <mergeCell ref="A2462:B2462"/>
+    <mergeCell ref="A2463:B2463"/>
+    <mergeCell ref="A2464:B2464"/>
+    <mergeCell ref="A2465:B2465"/>
+    <mergeCell ref="A2466:B2466"/>
+    <mergeCell ref="A2467:B2467"/>
+    <mergeCell ref="A2468:B2468"/>
+    <mergeCell ref="A2469:B2469"/>
+    <mergeCell ref="A2470:B2470"/>
+    <mergeCell ref="A2471:B2471"/>
+    <mergeCell ref="A2472:B2472"/>
+    <mergeCell ref="A2473:B2473"/>
+    <mergeCell ref="A2474:B2474"/>
+    <mergeCell ref="A2475:B2475"/>
+    <mergeCell ref="A2476:B2476"/>
+    <mergeCell ref="A2477:B2477"/>
+    <mergeCell ref="A2478:B2478"/>
+    <mergeCell ref="A2479:B2479"/>
+    <mergeCell ref="A2480:B2480"/>
+    <mergeCell ref="A2492:B2492"/>
+    <mergeCell ref="A2493:B2493"/>
+    <mergeCell ref="A2494:B2494"/>
+    <mergeCell ref="A2495:B2495"/>
+    <mergeCell ref="A2496:B2496"/>
+    <mergeCell ref="A2497:B2497"/>
+    <mergeCell ref="A2498:B2498"/>
+    <mergeCell ref="A2499:B2499"/>
+    <mergeCell ref="A2500:B2500"/>
+    <mergeCell ref="A2501:B2501"/>
+    <mergeCell ref="A2502:B2502"/>
+    <mergeCell ref="A2503:B2503"/>
+    <mergeCell ref="A2504:B2504"/>
+    <mergeCell ref="A2505:B2505"/>
+    <mergeCell ref="A2506:B2506"/>
+    <mergeCell ref="A2507:B2507"/>
+    <mergeCell ref="A2508:B2508"/>
+    <mergeCell ref="A2509:B2509"/>
+    <mergeCell ref="A2510:B2510"/>
+    <mergeCell ref="A2511:B2511"/>
+    <mergeCell ref="A2512:B2512"/>
+    <mergeCell ref="A2513:B2513"/>
+    <mergeCell ref="A2514:B2514"/>
+    <mergeCell ref="A2515:B2515"/>
+    <mergeCell ref="A2516:B2516"/>
+    <mergeCell ref="A2517:B2517"/>
+    <mergeCell ref="A2518:B2518"/>
+    <mergeCell ref="A2519:B2519"/>
+    <mergeCell ref="A2520:B2520"/>
     <mergeCell ref="A2543:B2543"/>
     <mergeCell ref="A2592:B2592"/>
     <mergeCell ref="A2593:B2593"/>
@@ -17806,474 +18274,6 @@
     <mergeCell ref="A2527:B2527"/>
     <mergeCell ref="A2528:B2528"/>
     <mergeCell ref="A2542:B2542"/>
-    <mergeCell ref="A2512:B2512"/>
-    <mergeCell ref="A2513:B2513"/>
-    <mergeCell ref="A2514:B2514"/>
-    <mergeCell ref="A2515:B2515"/>
-    <mergeCell ref="A2516:B2516"/>
-    <mergeCell ref="A2517:B2517"/>
-    <mergeCell ref="A2518:B2518"/>
-    <mergeCell ref="A2519:B2519"/>
-    <mergeCell ref="A2520:B2520"/>
-    <mergeCell ref="A2503:B2503"/>
-    <mergeCell ref="A2504:B2504"/>
-    <mergeCell ref="A2505:B2505"/>
-    <mergeCell ref="A2506:B2506"/>
-    <mergeCell ref="A2507:B2507"/>
-    <mergeCell ref="A2508:B2508"/>
-    <mergeCell ref="A2509:B2509"/>
-    <mergeCell ref="A2510:B2510"/>
-    <mergeCell ref="A2511:B2511"/>
-    <mergeCell ref="A2494:B2494"/>
-    <mergeCell ref="A2495:B2495"/>
-    <mergeCell ref="A2496:B2496"/>
-    <mergeCell ref="A2497:B2497"/>
-    <mergeCell ref="A2498:B2498"/>
-    <mergeCell ref="A2499:B2499"/>
-    <mergeCell ref="A2500:B2500"/>
-    <mergeCell ref="A2501:B2501"/>
-    <mergeCell ref="A2502:B2502"/>
-    <mergeCell ref="A2474:B2474"/>
-    <mergeCell ref="A2475:B2475"/>
-    <mergeCell ref="A2476:B2476"/>
-    <mergeCell ref="A2477:B2477"/>
-    <mergeCell ref="A2478:B2478"/>
-    <mergeCell ref="A2479:B2479"/>
-    <mergeCell ref="A2480:B2480"/>
-    <mergeCell ref="A2492:B2492"/>
-    <mergeCell ref="A2493:B2493"/>
-    <mergeCell ref="A2465:B2465"/>
-    <mergeCell ref="A2466:B2466"/>
-    <mergeCell ref="A2467:B2467"/>
-    <mergeCell ref="A2468:B2468"/>
-    <mergeCell ref="A2469:B2469"/>
-    <mergeCell ref="A2470:B2470"/>
-    <mergeCell ref="A2471:B2471"/>
-    <mergeCell ref="A2472:B2472"/>
-    <mergeCell ref="A2473:B2473"/>
-    <mergeCell ref="A2456:B2456"/>
-    <mergeCell ref="A2457:B2457"/>
-    <mergeCell ref="A2458:B2458"/>
-    <mergeCell ref="A2459:B2459"/>
-    <mergeCell ref="A2460:B2460"/>
-    <mergeCell ref="A2461:B2461"/>
-    <mergeCell ref="A2462:B2462"/>
-    <mergeCell ref="A2463:B2463"/>
-    <mergeCell ref="A2464:B2464"/>
-    <mergeCell ref="A2447:B2447"/>
-    <mergeCell ref="A2448:B2448"/>
-    <mergeCell ref="A2449:B2449"/>
-    <mergeCell ref="A2450:B2450"/>
-    <mergeCell ref="A2451:B2451"/>
-    <mergeCell ref="A2452:B2452"/>
-    <mergeCell ref="A2453:B2453"/>
-    <mergeCell ref="A2454:B2454"/>
-    <mergeCell ref="A2455:B2455"/>
-    <mergeCell ref="A2342:B2342"/>
-    <mergeCell ref="A2343:B2343"/>
-    <mergeCell ref="A2392:B2392"/>
-    <mergeCell ref="A2393:B2393"/>
-    <mergeCell ref="A2442:B2442"/>
-    <mergeCell ref="A2443:B2443"/>
-    <mergeCell ref="A2444:B2444"/>
-    <mergeCell ref="A2445:B2445"/>
-    <mergeCell ref="A2446:B2446"/>
-    <mergeCell ref="A2242:B2242"/>
-    <mergeCell ref="A2243:B2243"/>
-    <mergeCell ref="A2244:B2244"/>
-    <mergeCell ref="A2245:B2245"/>
-    <mergeCell ref="A2246:B2246"/>
-    <mergeCell ref="A2247:B2247"/>
-    <mergeCell ref="A2248:B2248"/>
-    <mergeCell ref="A2292:B2292"/>
-    <mergeCell ref="A2293:B2293"/>
-    <mergeCell ref="A2101:B2101"/>
-    <mergeCell ref="A2102:B2102"/>
-    <mergeCell ref="A2103:B2103"/>
-    <mergeCell ref="A2104:B2104"/>
-    <mergeCell ref="A2105:B2105"/>
-    <mergeCell ref="A2142:B2142"/>
-    <mergeCell ref="A2143:B2143"/>
-    <mergeCell ref="A2192:B2192"/>
-    <mergeCell ref="A2193:B2193"/>
-    <mergeCell ref="A2092:B2092"/>
-    <mergeCell ref="A2093:B2093"/>
-    <mergeCell ref="A2094:B2094"/>
-    <mergeCell ref="A2095:B2095"/>
-    <mergeCell ref="A2096:B2096"/>
-    <mergeCell ref="A2097:B2097"/>
-    <mergeCell ref="A2098:B2098"/>
-    <mergeCell ref="A2099:B2099"/>
-    <mergeCell ref="A2100:B2100"/>
-    <mergeCell ref="A1971:B1971"/>
-    <mergeCell ref="A1972:B1972"/>
-    <mergeCell ref="A1973:B1973"/>
-    <mergeCell ref="A1992:B1992"/>
-    <mergeCell ref="A1993:B1993"/>
-    <mergeCell ref="A1994:B1994"/>
-    <mergeCell ref="A1995:B1995"/>
-    <mergeCell ref="A2042:B2042"/>
-    <mergeCell ref="A2043:B2043"/>
-    <mergeCell ref="A1962:B1962"/>
-    <mergeCell ref="A1963:B1963"/>
-    <mergeCell ref="A1964:B1964"/>
-    <mergeCell ref="A1965:B1965"/>
-    <mergeCell ref="A1966:B1966"/>
-    <mergeCell ref="A1967:B1967"/>
-    <mergeCell ref="A1968:B1968"/>
-    <mergeCell ref="A1969:B1969"/>
-    <mergeCell ref="A1970:B1970"/>
-    <mergeCell ref="A1953:B1953"/>
-    <mergeCell ref="A1954:B1954"/>
-    <mergeCell ref="A1955:B1955"/>
-    <mergeCell ref="A1956:B1956"/>
-    <mergeCell ref="A1957:B1957"/>
-    <mergeCell ref="A1958:B1958"/>
-    <mergeCell ref="A1959:B1959"/>
-    <mergeCell ref="A1960:B1960"/>
-    <mergeCell ref="A1961:B1961"/>
-    <mergeCell ref="A1944:B1944"/>
-    <mergeCell ref="A1945:B1945"/>
-    <mergeCell ref="A1946:B1946"/>
-    <mergeCell ref="A1947:B1947"/>
-    <mergeCell ref="A1948:B1948"/>
-    <mergeCell ref="A1949:B1949"/>
-    <mergeCell ref="A1950:B1950"/>
-    <mergeCell ref="A1951:B1951"/>
-    <mergeCell ref="A1952:B1952"/>
-    <mergeCell ref="A1820:B1820"/>
-    <mergeCell ref="A1821:B1821"/>
-    <mergeCell ref="A1822:B1822"/>
-    <mergeCell ref="A1842:B1842"/>
-    <mergeCell ref="A1843:B1843"/>
-    <mergeCell ref="A1892:B1892"/>
-    <mergeCell ref="A1893:B1893"/>
-    <mergeCell ref="A1942:B1942"/>
-    <mergeCell ref="A1943:B1943"/>
-    <mergeCell ref="A1811:B1811"/>
-    <mergeCell ref="A1812:B1812"/>
-    <mergeCell ref="A1813:B1813"/>
-    <mergeCell ref="A1814:B1814"/>
-    <mergeCell ref="A1815:B1815"/>
-    <mergeCell ref="A1816:B1816"/>
-    <mergeCell ref="A1817:B1817"/>
-    <mergeCell ref="A1818:B1818"/>
-    <mergeCell ref="A1819:B1819"/>
-    <mergeCell ref="A1802:B1802"/>
-    <mergeCell ref="A1803:B1803"/>
-    <mergeCell ref="A1804:B1804"/>
-    <mergeCell ref="A1805:B1805"/>
-    <mergeCell ref="A1806:B1806"/>
-    <mergeCell ref="A1807:B1807"/>
-    <mergeCell ref="A1808:B1808"/>
-    <mergeCell ref="A1809:B1809"/>
-    <mergeCell ref="A1810:B1810"/>
-    <mergeCell ref="A1793:B1793"/>
-    <mergeCell ref="A1794:B1794"/>
-    <mergeCell ref="A1795:B1795"/>
-    <mergeCell ref="A1796:B1796"/>
-    <mergeCell ref="A1797:B1797"/>
-    <mergeCell ref="A1798:B1798"/>
-    <mergeCell ref="A1799:B1799"/>
-    <mergeCell ref="A1800:B1800"/>
-    <mergeCell ref="A1801:B1801"/>
-    <mergeCell ref="A1760:B1760"/>
-    <mergeCell ref="A1761:B1761"/>
-    <mergeCell ref="A1762:B1762"/>
-    <mergeCell ref="A1763:B1763"/>
-    <mergeCell ref="A1764:B1764"/>
-    <mergeCell ref="A1765:B1765"/>
-    <mergeCell ref="A1766:B1766"/>
-    <mergeCell ref="A1767:B1767"/>
-    <mergeCell ref="A1792:B1792"/>
-    <mergeCell ref="A1751:B1751"/>
-    <mergeCell ref="A1752:B1752"/>
-    <mergeCell ref="A1753:B1753"/>
-    <mergeCell ref="A1754:B1754"/>
-    <mergeCell ref="A1755:B1755"/>
-    <mergeCell ref="A1756:B1756"/>
-    <mergeCell ref="A1757:B1757"/>
-    <mergeCell ref="A1758:B1758"/>
-    <mergeCell ref="A1759:B1759"/>
-    <mergeCell ref="A1742:B1742"/>
-    <mergeCell ref="A1743:B1743"/>
-    <mergeCell ref="A1744:B1744"/>
-    <mergeCell ref="A1745:B1745"/>
-    <mergeCell ref="A1746:B1746"/>
-    <mergeCell ref="A1747:B1747"/>
-    <mergeCell ref="A1748:B1748"/>
-    <mergeCell ref="A1749:B1749"/>
-    <mergeCell ref="A1750:B1750"/>
-    <mergeCell ref="A1678:B1678"/>
-    <mergeCell ref="A1679:B1679"/>
-    <mergeCell ref="A1680:B1680"/>
-    <mergeCell ref="A1681:B1681"/>
-    <mergeCell ref="A1682:B1682"/>
-    <mergeCell ref="A1683:B1683"/>
-    <mergeCell ref="A1684:B1684"/>
-    <mergeCell ref="A1692:B1692"/>
-    <mergeCell ref="A1693:B1693"/>
-    <mergeCell ref="A1669:B1669"/>
-    <mergeCell ref="A1670:B1670"/>
-    <mergeCell ref="A1671:B1671"/>
-    <mergeCell ref="A1672:B1672"/>
-    <mergeCell ref="A1673:B1673"/>
-    <mergeCell ref="A1674:B1674"/>
-    <mergeCell ref="A1675:B1675"/>
-    <mergeCell ref="A1676:B1676"/>
-    <mergeCell ref="A1677:B1677"/>
-    <mergeCell ref="A1660:B1660"/>
-    <mergeCell ref="A1661:B1661"/>
-    <mergeCell ref="A1662:B1662"/>
-    <mergeCell ref="A1663:B1663"/>
-    <mergeCell ref="A1664:B1664"/>
-    <mergeCell ref="A1665:B1665"/>
-    <mergeCell ref="A1666:B1666"/>
-    <mergeCell ref="A1667:B1667"/>
-    <mergeCell ref="A1668:B1668"/>
-    <mergeCell ref="A1651:B1651"/>
-    <mergeCell ref="A1652:B1652"/>
-    <mergeCell ref="A1653:B1653"/>
-    <mergeCell ref="A1654:B1654"/>
-    <mergeCell ref="A1655:B1655"/>
-    <mergeCell ref="A1656:B1656"/>
-    <mergeCell ref="A1657:B1657"/>
-    <mergeCell ref="A1658:B1658"/>
-    <mergeCell ref="A1659:B1659"/>
-    <mergeCell ref="A1642:B1642"/>
-    <mergeCell ref="A1643:B1643"/>
-    <mergeCell ref="A1644:B1644"/>
-    <mergeCell ref="A1645:B1645"/>
-    <mergeCell ref="A1646:B1646"/>
-    <mergeCell ref="A1647:B1647"/>
-    <mergeCell ref="A1648:B1648"/>
-    <mergeCell ref="A1649:B1649"/>
-    <mergeCell ref="A1650:B1650"/>
-    <mergeCell ref="A1579:B1579"/>
-    <mergeCell ref="A1580:B1580"/>
-    <mergeCell ref="A1581:B1581"/>
-    <mergeCell ref="A1582:B1582"/>
-    <mergeCell ref="A1583:B1583"/>
-    <mergeCell ref="A1584:B1584"/>
-    <mergeCell ref="A1585:B1585"/>
-    <mergeCell ref="A1592:B1592"/>
-    <mergeCell ref="A1593:B1593"/>
-    <mergeCell ref="A1570:B1570"/>
-    <mergeCell ref="A1571:B1571"/>
-    <mergeCell ref="A1572:B1572"/>
-    <mergeCell ref="A1573:B1573"/>
-    <mergeCell ref="A1574:B1574"/>
-    <mergeCell ref="A1575:B1575"/>
-    <mergeCell ref="A1576:B1576"/>
-    <mergeCell ref="A1577:B1577"/>
-    <mergeCell ref="A1578:B1578"/>
-    <mergeCell ref="A1561:B1561"/>
-    <mergeCell ref="A1562:B1562"/>
-    <mergeCell ref="A1563:B1563"/>
-    <mergeCell ref="A1564:B1564"/>
-    <mergeCell ref="A1565:B1565"/>
-    <mergeCell ref="A1566:B1566"/>
-    <mergeCell ref="A1567:B1567"/>
-    <mergeCell ref="A1568:B1568"/>
-    <mergeCell ref="A1569:B1569"/>
-    <mergeCell ref="A1552:B1552"/>
-    <mergeCell ref="A1553:B1553"/>
-    <mergeCell ref="A1554:B1554"/>
-    <mergeCell ref="A1555:B1555"/>
-    <mergeCell ref="A1556:B1556"/>
-    <mergeCell ref="A1557:B1557"/>
-    <mergeCell ref="A1558:B1558"/>
-    <mergeCell ref="A1559:B1559"/>
-    <mergeCell ref="A1560:B1560"/>
-    <mergeCell ref="A1543:B1543"/>
-    <mergeCell ref="A1544:B1544"/>
-    <mergeCell ref="A1545:B1545"/>
-    <mergeCell ref="A1546:B1546"/>
-    <mergeCell ref="A1547:B1547"/>
-    <mergeCell ref="A1548:B1548"/>
-    <mergeCell ref="A1549:B1549"/>
-    <mergeCell ref="A1550:B1550"/>
-    <mergeCell ref="A1551:B1551"/>
-    <mergeCell ref="A1342:B1342"/>
-    <mergeCell ref="A1343:B1343"/>
-    <mergeCell ref="A1392:B1392"/>
-    <mergeCell ref="A1393:B1393"/>
-    <mergeCell ref="A1442:B1442"/>
-    <mergeCell ref="A1443:B1443"/>
-    <mergeCell ref="A1492:B1492"/>
-    <mergeCell ref="A1493:B1493"/>
-    <mergeCell ref="A1542:B1542"/>
-    <mergeCell ref="A1093:B1093"/>
-    <mergeCell ref="A1142:B1142"/>
-    <mergeCell ref="A1143:B1143"/>
-    <mergeCell ref="A1192:B1192"/>
-    <mergeCell ref="A1193:B1193"/>
-    <mergeCell ref="A1242:B1242"/>
-    <mergeCell ref="A1243:B1243"/>
-    <mergeCell ref="A1292:B1292"/>
-    <mergeCell ref="A1293:B1293"/>
-    <mergeCell ref="A892:B892"/>
-    <mergeCell ref="A893:B893"/>
-    <mergeCell ref="A942:B942"/>
-    <mergeCell ref="A943:B943"/>
-    <mergeCell ref="A992:B992"/>
-    <mergeCell ref="A993:B993"/>
-    <mergeCell ref="A1042:B1042"/>
-    <mergeCell ref="A1043:B1043"/>
-    <mergeCell ref="A1092:B1092"/>
-    <mergeCell ref="A865:B865"/>
-    <mergeCell ref="A866:B866"/>
-    <mergeCell ref="A867:B867"/>
-    <mergeCell ref="A868:B868"/>
-    <mergeCell ref="A869:B869"/>
-    <mergeCell ref="A870:B870"/>
-    <mergeCell ref="A871:B871"/>
-    <mergeCell ref="A872:B872"/>
-    <mergeCell ref="A873:B873"/>
-    <mergeCell ref="A856:B856"/>
-    <mergeCell ref="A857:B857"/>
-    <mergeCell ref="A858:B858"/>
-    <mergeCell ref="A859:B859"/>
-    <mergeCell ref="A860:B860"/>
-    <mergeCell ref="A861:B861"/>
-    <mergeCell ref="A862:B862"/>
-    <mergeCell ref="A863:B863"/>
-    <mergeCell ref="A864:B864"/>
-    <mergeCell ref="A847:B847"/>
-    <mergeCell ref="A848:B848"/>
-    <mergeCell ref="A849:B849"/>
-    <mergeCell ref="A850:B850"/>
-    <mergeCell ref="A851:B851"/>
-    <mergeCell ref="A852:B852"/>
-    <mergeCell ref="A853:B853"/>
-    <mergeCell ref="A854:B854"/>
-    <mergeCell ref="A855:B855"/>
-    <mergeCell ref="A742:B742"/>
-    <mergeCell ref="A743:B743"/>
-    <mergeCell ref="A792:B792"/>
-    <mergeCell ref="A793:B793"/>
-    <mergeCell ref="A842:B842"/>
-    <mergeCell ref="A843:B843"/>
-    <mergeCell ref="A844:B844"/>
-    <mergeCell ref="A845:B845"/>
-    <mergeCell ref="A846:B846"/>
-    <mergeCell ref="A493:B493"/>
-    <mergeCell ref="A542:B542"/>
-    <mergeCell ref="A543:B543"/>
-    <mergeCell ref="A592:B592"/>
-    <mergeCell ref="A593:B593"/>
-    <mergeCell ref="A642:B642"/>
-    <mergeCell ref="A643:B643"/>
-    <mergeCell ref="A692:B692"/>
-    <mergeCell ref="A693:B693"/>
-    <mergeCell ref="A426:B426"/>
-    <mergeCell ref="A427:B427"/>
-    <mergeCell ref="A428:B428"/>
-    <mergeCell ref="A429:B429"/>
-    <mergeCell ref="A430:B430"/>
-    <mergeCell ref="A431:B431"/>
-    <mergeCell ref="A442:B442"/>
-    <mergeCell ref="A443:B443"/>
-    <mergeCell ref="A492:B492"/>
-    <mergeCell ref="A417:B417"/>
-    <mergeCell ref="A418:B418"/>
-    <mergeCell ref="A419:B419"/>
-    <mergeCell ref="A420:B420"/>
-    <mergeCell ref="A421:B421"/>
-    <mergeCell ref="A422:B422"/>
-    <mergeCell ref="A423:B423"/>
-    <mergeCell ref="A424:B424"/>
-    <mergeCell ref="A425:B425"/>
-    <mergeCell ref="A408:B408"/>
-    <mergeCell ref="A409:B409"/>
-    <mergeCell ref="A410:B410"/>
-    <mergeCell ref="A411:B411"/>
-    <mergeCell ref="A412:B412"/>
-    <mergeCell ref="A413:B413"/>
-    <mergeCell ref="A414:B414"/>
-    <mergeCell ref="A415:B415"/>
-    <mergeCell ref="A416:B416"/>
-    <mergeCell ref="A399:B399"/>
-    <mergeCell ref="A400:B400"/>
-    <mergeCell ref="A401:B401"/>
-    <mergeCell ref="A402:B402"/>
-    <mergeCell ref="A403:B403"/>
-    <mergeCell ref="A404:B404"/>
-    <mergeCell ref="A405:B405"/>
-    <mergeCell ref="A406:B406"/>
-    <mergeCell ref="A407:B407"/>
-    <mergeCell ref="A342:B342"/>
-    <mergeCell ref="A343:B343"/>
-    <mergeCell ref="A392:B392"/>
-    <mergeCell ref="A393:B393"/>
-    <mergeCell ref="A394:B394"/>
-    <mergeCell ref="A395:B395"/>
-    <mergeCell ref="A396:B396"/>
-    <mergeCell ref="A397:B397"/>
-    <mergeCell ref="A398:B398"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="A242:B242"/>
-    <mergeCell ref="A243:B243"/>
-    <mergeCell ref="A292:B292"/>
-    <mergeCell ref="A293:B293"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -18285,10 +18285,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E113E54-E5F9-40CE-8717-0C3FEAB1378C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B18FBE-20F0-4EBD-A19D-F52FB3CBCCA3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>

</xml_diff>